<commit_message>
Add filename revisioning and template validation tests
- Implemented a function to generate filenames with revision indicators in the organize_lots and template_filler modules.
- Updated the template filling logic to include revised filenames.
- Created a new script to validate the template structure and content.
- Added tests to ensure proper functionality of the new features.
</commit_message>
<xml_diff>
--- a/tests/fixtures/template_exemplo.xlsx
+++ b/tests/fixtures/template_exemplo.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,6 +468,13 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>FIM</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>